<commit_message>
feat: :art: Se agrego paginacion
</commit_message>
<xml_diff>
--- a/mercadolibre.xlsx
+++ b/mercadolibre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Laptop Lenovo 15.6 Fhd, Pentium Silver, 4gb Ram, 128gbemmc Color Negro</t>
+          <t>HP Laptop 14-ew1000la Intel Core Ultra 5 16GB RAM 512GB SSD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4,299</t>
+          <t>21,999</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -490,12 +490,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Notebook Aspire 5 A515-58M 15.6" negro 16GB de Ram - 512GB SSD - Intel Core i5</t>
+          <t>Notebook Asus Vivobook Intel Core I3 1215u, 8gb De Ram, 128gb Ssd, Full Hd, Windows 11 Home</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12,789</t>
+          <t>6,190</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,7 +505,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -517,12 +517,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Laptop Lenovo Ideapad Celeron 4gb + 128ssd + Office Regalo Color Gris</t>
+          <t>Laptop Acer Aspire 3 15.6 Ryzen 7, 16gb/512gb, Windows 11 Color Plateado</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3,649</t>
+          <t>7,999</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -544,12 +544,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Laptop Hp 14 Dq0509la Celeron N4120 Ram 4gb Ssd 128gb</t>
+          <t>Laptop 15.6in Notebook Intel Celeron N5095 16g Ram 256g Ssd Color Plateado</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4,189</t>
+          <t>5,299</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -559,7 +559,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -571,12 +571,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Notebook 15-dw1083wm 15.6" scarlet red 4GB de Ram - 128GB SSD - Intel Pentium Gold</t>
+          <t>Notebook N5095 15.6" gris 8GB de Ram - 256GB SSD - Intel Celeron</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6,499</t>
+          <t>6,941</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -598,12 +598,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Laptop Dell Inspiron 15 Ryzen 5 8gb Ddr5 512gb Ssd + Mouse</t>
+          <t>Laptop Lenovo Ideapad Celeron 4gb + 128ssd + Office Regalo Color Gris</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7,499</t>
+          <t>3,699</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -625,12 +625,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Laptop Acer Aspire 3 15.6 Ryzen 7, 16gb/512gb, Windows 11 Color Plateado</t>
+          <t>Apple MacBook Air (13 pulgadas, 2020, Chip M1, 256 GB de SSD, 8 GB de RAM) - Gris espacial - Distribuidor Autorizado</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7,999</t>
+          <t>11,999</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -652,12 +652,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Laptop Asus Vivobook F15 15.6 Core I7 1255u 16g 512g Ssd W11 Color Azul</t>
+          <t>Laptop gamer Thunderobot 911MT 12th Intel Core i7 12650H 16GB de RAM 512GB SSD, NVIDIA GeForce RTX 3050 165 Hz 1920x1080px Windows 11 Pro</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>12,656</t>
+          <t>15,762</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -679,12 +679,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Laptop Hp 14-dq0526la Intel Celeron 4gb 128gb + Impresora</t>
+          <t>Laptop Acer Etbook Intel Core I5-12450h 16gb 512gb Ssd Win11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5,199</t>
+          <t>8,618</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Laptop Hp 240 G9 Intel Ci3-1215u 8gb 256gb Ssd + Regalos</t>
+          <t>Portátil Vanwin 11.6 Intel 8gb Ram 256g Rom Windows 11 Gris</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5,979</t>
+          <t>3,855</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -721,10 +721,550 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HP Laptop 14-ew1000la Intel Core Ultra 5 16GB RAM 512GB SSD</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>21,999</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Laptop Acer Etbook Intel Core I5-12450h 16gb 512gb Ssd Win11</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>8,618</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Portátil Vanwin 11.6 Intel 8gb Ram 256g Rom Windows 11 Gris</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>3,855</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad Slim 3 15.6'' Ci5 8gb + 512gb Ssd</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>8,799</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Ultrabook Win VNJH1601-3 16" plateado 16GB de Ram - 1TB SSD - Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>13,635</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Lenovo T490 Thinkpad Core I5 8va 8gb 256 Ssd 14 Fhd W10 Pro</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>4,317</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Notebook V-Series V14 14" black 4GB de Ram - 128GB SSD - Intel Celeron</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3,801</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Apple MacBook Air (13 pulgadas, 2020, Chip M1, 256 GB de SSD, 8 GB de RAM) - Gris espacial</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>12,199</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Laptop Moderness Lt1505 16+512g 15.6 1920*1080p Windows 11</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5,499</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Notebook Asus Vivobook Intel Core I3 1215u, 8gb De Ram, 128gb Ssd, Full Hd, Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6,190</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ordenador Portátil Windows 11 Intel Core I7 16gb+1tb Ssd</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10,566</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Notebook N5095 15.6" gris 8GB de Ram - 256GB SSD - Intel Celeron</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>6,941</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Laptop 15.6inch Intel 2 En 1 Ddr4 De 16gb Ram 512 Gb</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>5,308</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Notebook Stream 14-cf2112wm rosa 4GB de Ram - 64GB SSD - Intel Celeron</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>4,211</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Notebook Acer Aspire 3 Ryzen 5 7520u 512g 16g 15.6 Touch Color Gris</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>10,036</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad Slim 3 Core I7 Ram 16gb Ssd 1tb W11h Color Gris</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16,799</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad 15.6 Ryzen 3 7320u 8gb 256gb ssd</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>6,799</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Laptop Asus 15-x5ja Core I3-1005, 512gb Ssd 8gb Ram, Fhd</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>5,871</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Notebook Msi Amd Ryzen 5-7530u 16gb 512gb 14'' Fhd Black Color Negro</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>11,399</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Yinkuu Laptop Intel Celeron 16gb+512gb Ssd 15.6 Uhd 4k</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>5,129</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>mercadolibre</t>
         </is>

</xml_diff>

<commit_message>
refactor: :fire: Se funciono funcion de lectura de tabla y archivos en una sola función
</commit_message>
<xml_diff>
--- a/mercadolibre.xlsx
+++ b/mercadolibre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,12 +517,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Laptop Acer Aspire 3 15.6 Ryzen 7, 16gb/512gb, Windows 11 Color Plateado</t>
+          <t>Apple MacBook Air (13 pulgadas, 2020, Chip M1, 256 GB de SSD, 8 GB de RAM) - Gris espacial - Distribuidor Autorizado</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7,999</t>
+          <t>11,999</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -598,12 +598,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Laptop Lenovo Ideapad Celeron 4gb + 128ssd + Office Regalo Color Gris</t>
+          <t>Laptop Acer Aspire 3 15.6 Ryzen 7, 16gb/512gb, Windows 11 Color Plateado</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3,699</t>
+          <t>7,999</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -625,12 +625,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Apple MacBook Air (13 pulgadas, 2020, Chip M1, 256 GB de SSD, 8 GB de RAM) - Gris espacial - Distribuidor Autorizado</t>
+          <t>Laptop Lenovo Ideapad Celeron 4gb + 128ssd + Office Regalo Color Gris</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11,999</t>
+          <t>3,699</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -652,12 +652,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Laptop gamer Thunderobot 911MT 12th Intel Core i7 12650H 16GB de RAM 512GB SSD, NVIDIA GeForce RTX 3050 165 Hz 1920x1080px Windows 11 Pro</t>
+          <t>Laptop Dell 3525, 15.6 Fhd , Ryzen 7, 16gb, 1tb Ssd, W11h Color Black</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15,762</t>
+          <t>10,899</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -679,12 +679,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Laptop Acer Etbook Intel Core I5-12450h 16gb 512gb Ssd Win11</t>
+          <t>Laptop Moderness Lt1505 16+512g 15.6 1920*1080p Windows 11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8,618</t>
+          <t>5,499</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Portátil Vanwin 11.6 Intel 8gb Ram 256g Rom Windows 11 Gris</t>
+          <t>Notebook Msi Amd Ryzen 5-7530u 16gb 512gb 14'' Fhd Black Color Negro</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3,855</t>
+          <t>11,399</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -733,12 +733,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HP Laptop 14-ew1000la Intel Core Ultra 5 16GB RAM 512GB SSD</t>
+          <t>Laptop Chuwi HeroBook Pro space gray 14.1", Intel Celeron N4020 8GB de RAM 256GB SSD, Intel UHD Graphics 600 1920x1080px Windows 11 Home</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21,999</t>
+          <t>3,931</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -760,12 +760,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Laptop Acer Etbook Intel Core I5-12450h 16gb 512gb Ssd Win11</t>
+          <t>Laptop Hp 245 G9 Amd Ryzen 3 3250u 8gb Ssd 256gb 14 Hd W11h Color Negro</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8,618</t>
+          <t>5,298</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -787,12 +787,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Portátil Vanwin 11.6 Intel 8gb Ram 256g Rom Windows 11 Gris</t>
+          <t>Laptop Intel Celeron 2 en 1 Notebook DDR4 16 GB RAM 512 GB SSD 15.6' Plateado 1920 px x 1080 px Windows 11</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3,855</t>
+          <t>5,102</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -814,12 +814,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Laptop Lenovo Ideapad Slim 3 15.6'' Ci5 8gb + 512gb Ssd</t>
+          <t>Notebook Laptop Geobook 2E 12.5" negro 4GB de Ram - 64GB SSD - Intel Celeron</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8,799</t>
+          <t>2,618</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -841,12 +841,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ultrabook Win VNJH1601-3 16" plateado 16GB de Ram - 1TB SSD - Intel Core i7</t>
+          <t>Laptop gamer Thunderobot 911MT 12th Intel Core i7 12650H 16GB de RAM 512GB SSD, NVIDIA GeForce RTX 3050 165 Hz 1920x1080px Windows 11 Pro</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>13,635</t>
+          <t>15,762</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -868,12 +868,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Lenovo T490 Thinkpad Core I5 8va 8gb 256 Ssd 14 Fhd W10 Pro</t>
+          <t>Notebook Gateway 14.1' Fhd Core I3 128gb Ssd 4gb Ram W10 Amv Color Azul</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4,317</t>
+          <t>3,999</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -895,12 +895,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Notebook V-Series V14 14" black 4GB de Ram - 128GB SSD - Intel Celeron</t>
+          <t>Notebook D-1420 14.1" gris 8GB de Ram - 256GB SSD - Intel Celeron</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3,801</t>
+          <t>4,193</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -910,7 +910,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -922,12 +922,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Apple MacBook Air (13 pulgadas, 2020, Chip M1, 256 GB de SSD, 8 GB de RAM) - Gris espacial</t>
+          <t>Laptop Lenovo Ideapad Slim 5, Amd Ryzen 5 7530u, 8gb Ram, 512gb Ssd, Windows 11 Home 64-bit, 14 Pulgadas Wuxga, Teclado En Español Retroiluminado, Gris</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>12,199</t>
+          <t>8,759</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -937,7 +937,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -949,12 +949,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Laptop Moderness Lt1505 16+512g 15.6 1920*1080p Windows 11</t>
+          <t>Laptop Hp 245 G9 Amd Ryzen 3 3250u Hasta 3,5 Ghz, Memoria Ram De 16 Gb Ddr4, Ssd 256 Gb, Windows 11 Home 64-bit, Teclado En Español, 14 Pulgadas, Negro.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5,499</t>
+          <t>5,617</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -976,12 +976,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Notebook Asus Vivobook Intel Core I3 1215u, 8gb De Ram, 128gb Ssd, Full Hd, Windows 11 Home</t>
+          <t>Notebook Education Maestro E-Book 11.6" gray 4GB de Ram - 64GB SSD - Intel Celeron</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6,190</t>
+          <t>2,889</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1003,12 +1003,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ordenador Portátil Windows 11 Intel Core I7 16gb+1tb Ssd</t>
+          <t>Laptop Hp 240 G9 Intel Core I3 1215u 512gb Ssd 16gb Ram 1366x768px Windows 11 Home + Antivirus Norton 360</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>10,566</t>
+          <t>6,429</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1030,12 +1030,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Notebook N5095 15.6" gris 8GB de Ram - 256GB SSD - Intel Celeron</t>
+          <t>Laptop Asus Asus Tuf Gaming A15 Amd R5 Rtx2050 16gb 512gb Color Negro</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6,941</t>
+          <t>13,999</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1057,12 +1057,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Laptop 15.6inch Intel 2 En 1 Ddr4 De 16gb Ram 512 Gb</t>
+          <t>Laptop Hp 240 G8 Intel Core I3-1115g4 16gb De Ram Ddr4 256gb Ssd Sólido, Windows 11 Home 64 Bits, Teclado En Español.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5,308</t>
+          <t>5,999</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1084,12 +1084,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Notebook Stream 14-cf2112wm rosa 4GB de Ram - 64GB SSD - Intel Celeron</t>
+          <t>Laptop Dell Inspiron 3520 Core I3 1215u Ram 8gb Ssd 512gb Color Plateado</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4,211</t>
+          <t>6,899</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1111,12 +1111,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Notebook Acer Aspire 3 Ryzen 5 7520u 512g 16g 15.6 Touch Color Gris</t>
+          <t>Notebook Victus 15-fb1013dx 15.6" gris 16GB de Ram - 512GB SSD - AMD Ryzen 5</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>10,036</t>
+          <t>13,919</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1138,12 +1138,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Laptop Lenovo Ideapad Slim 3 Core I7 Ram 16gb Ssd 1tb W11h Color Gris</t>
+          <t>Laptop HP 14-dq2531la Intel Core i3 16 GB 512 GB 14 pulgadas</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16,799</t>
+          <t>7,874</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1165,12 +1165,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Laptop Lenovo Ideapad 15.6 Ryzen 3 7320u 8gb 256gb ssd</t>
+          <t>Laptop HP AMD Ryzen 3 5300U 16GB 256GB SSD Pantalla Touch 14" Mouse DXT</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>6,799</t>
+          <t>6,249</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1192,12 +1192,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Laptop Asus 15-x5ja Core I3-1005, 512gb Ssd 8gb Ram, Fhd</t>
+          <t>Notebook 240 G9 14" plateado 8GB de Ram - 256GB SSD - Intel Celeron</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5,871</t>
+          <t>5,105</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1219,12 +1219,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Notebook Msi Amd Ryzen 5-7530u 16gb 512gb 14'' Fhd Black Color Negro</t>
+          <t>Portátil Ultrabook L16AIR 16" plateado 16GB de Ram 512GB SSD AMD Ryzen 7</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>11,399</t>
+          <t>13,907</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1246,12 +1246,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Yinkuu Laptop Intel Celeron 16gb+512gb Ssd 15.6 Uhd 4k</t>
+          <t>Laptop Lenovo Ideapad Slim 3 Intel Core I3-1305u 13.a Generación, 8 Gb Ram, 256 Gb Ssd, 15.6 Pulgadas Full Hd, Intel Uhd Graphics , Windows 11 Home 64 Bits, Teclado En Español.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5,129</t>
+          <t>6,732</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1261,10 +1261,2197 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Ultrabook Win VNJH1601-3 16" plateado 16GB de Ram - 1TB SSD - Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>13,635</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Lenovo T490 Thinkpad Core I5 8va 8gb 256 Ssd 14 Fhd W10 Pro</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>4,317</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Apple MacBook Air (13 pulgadas, 2020, Chip M1, 256 GB de SSD, 8 GB de RAM) - Gris espacial</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>12,199</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>porta lap top Chuwi GemiBook Plus plateada 15.6" , Intel N100 16GB de RAM 512GB SSD, Intel UHD Graphics 1920x1080px Windows 11 Home Color gris</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>5,569</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Notebook Pavilion 15-eg0510la 15.6" azul 12GB de Ram - 512GB SSD - Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>8,499</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Laptop Hp 14-dq0518la Celeron N4120 Ram 4gb Ssd 128gb W11h Color Plateado</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>4,189</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo V14 G3 Iap: Intel Core i3 1215U, RAM 8GB DDR4, SSD 256GB, Pantalla LED de 14", Windows 11 Home.</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>5,429</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Laptop Hp 255 G8 Amd Ryzen 5-5500u 8gb 256gb Ssd W11h Color Negro</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>6,719</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Laptop Hp 245 G9 Amd Ryzen 3 3250u Memoria Ram 8gb Ssd 256gb Windows 11 Home 64-bit, Teclado En Español, 14 Pulgadas, Negro.</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>5,355</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Laptop 2 en 1 Intel Celeron DDR4 16GB RAM 512GB SSD 15.6'' 4K FHD IPS Windows 11 Pro Ultrabook 2.4G/5G Dual Wifi</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>5,367</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Laptop Asus Vivobook Go 15 R5 16gb 512gb + Mochila + Mouse</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>9,699</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Laptop 2 En 1 Intel Celeron N5095 16gb Ram 256gb Ssd 15.6in</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>5,398</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Wozifan Laptop 14 Windows 6gb+scalable Ssd N4020 Wifi+mouse</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>3,283</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Laptop Dell Inspiron 3535 Ryzen 5 7520u 512gb Ssd 8gb Ddr5 Color Plateado</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>7,124</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Laptop 8gb Ram+1tb Ssd Celeron J4105 14.1' Windows 11 Intel</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>3,914</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Laptop MSI Gamer Thin GF63 15.6" 16GB de Ram 512GB SSD Intel Core i5 11400H Black</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>14,099</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Laptop Chuwi Corebook X 14 Intel Core I5, 16gb De Ram 512gb Ssd,4k Windows 11 Gris,teclado Iluminado&amp;con Ventilador</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>6,416</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Laptop Hp 240 G8 5t9j9lt 14 Pulgadas Intel Core I3 1115g4 Memoria Ram 8gb Ssd 256gb Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>5,227</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Laptop Hp 240 G9 Intel Core I3-1215u 12va Generación, 8gb Ram, 256gb Ssd, Windows 11 Home, 14 Pulgadas Hd, Teclado En Español.</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>5,799</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Laptop Huawei Matebook D15 Core I5 11.5th 8gb +512ssd Color Plateado</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>10,999</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Laptop Hp 255 G8 Ryzen 5 5500u 16gb M.2 256gb Ssd W11h 15.6 Color Negro</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>7,899</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Laptop  HP 15-ef2507la AMD Ryzen 5, 8 GB RAMM, 512 GB SSD, 15.6", HD</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>7,499</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Laptop 2 En 1 Intel I7 9750h 16gb Ram 512gb Ssd 15.6in Color Gris</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>8,120</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Laptop Huawei Matebook D15 Ryzen 7 16GB Ram y 512GB SSD W11 Color Gris</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>12,999</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Laptop Celeron N4000 8gb Ram 256gb Ssd 14 Pulgadas Notebook</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>3,631</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Gateway Notebook 11.6 Touch 2-in-1 N4020, 4gb, 64gb W10 Blu Color Azul</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2,999</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>HP Laptop 14-ew1000la Intel Core Ultra 5 16GB RAM 512GB SSD</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>21,999</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Laptop Moderness Lt1505 16+512g 15.6 1920*1080p Windows 11</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>5,499</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Notebook Asus Vivobook Intel Core I3 1215u, 8gb De Ram, 128gb Ssd, Full Hd, Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>6,190</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Laptop Asus Vivobook Intel Core I3 1215u 16gb Ddr4 512gb Ssd 15.6 Windows 11 Home + Mouse Dxt</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>7,499</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>3.7</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Laptop HP Victus Gaming Laptop 15-fb1013dx 15.6'' AMD Ryzen 5 7535hs 8 Ram 512 Ssd Rtx 2050 - Color Mica Silver</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>15,168</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Laptop Samsung 4 Chromebook Celeron 4gb 16gb Emmc Google</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1,398</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Laptop Hp 14 Dq0509la Celeron N4120 Ram 4gb Ssd 128gb</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>4,189</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Laptop Hp 240 G9: Intel Core I5-1235u (12 Va Gen), 8gb Ram, Ssd De 512gb, Pantalla De 14 Led, Video Iris Xe Graphics, W11h, Teclado En Español.</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>7,799</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Laptop 15.6in Notebook Intel Celeron N5095 16g Ram 256g Ssd Color Plateado</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>5,299</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Laptop Acer Etbook Intel Core I5-12450h 16gb 512gb Ssd Win11</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>8,618</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Slim 3 15abr8 Ryzen 7-7730u 512gb Ssd 16gb Ram Color Artic Grey</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>10,247</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>14.1'' Laptop 8 Ram+512gb Ssd Intel Celeron N4000 Windows 11</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>3,599</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Hp 15.6'' Intel I7 Ram 16gb Ssd 512gb Touchscreen Color Plateado</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>14,261</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Laptop Hp 240 Core I3 1115g4 16gb 512gb Ssd M.2 14 W11h Color Negro</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>5,999</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Alienware M16 Qhd+ 165hz Intel I7 16gb Ram Rtx 4070 1tb Ssd Color Dark Metallic Moon</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>39,899</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Notebook IdeaPad Ideapad 3 15.6" táctil azul 8GB de Ram - 512GB SSD - Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>8,637</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Notebook W7 14" dorado 6GB de Ram - 256GB SSD - Intel Celeron</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>3,711</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad Slim 3 Core I7 Ram 16gb Ssd 1tb W11h Color Gris</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>16,799</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad 15.6 Ryzen 3 7320u 8gb 256gb ssd</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>6,799</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Notebook Inspiron 3520 15.6" negro 8GB de Ram - 256GB SSD - Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>7,929</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Laptop Hp 255 G8 Ryzen 5 5500u 16gb 256gb Ssd 15.6 + Mouse</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>7,399</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Laptop Hp 14-dq0762dx Celeron 4gb 128gb Ssd Rosa</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>4,439</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Notebook 15-dy2073dx 15.6" táctil plata natural 16GB de Ram - 512GB SSD - Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>12,884</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Notebook 14 N4000 4gb + 64gb Emmc Ssd / Hp Stream W10 Color Azul</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>3,685</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Laptop Dell Barata I5 8va 8gb 512 Ssd Batería Nueva + Regalo</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>4,317</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Notebook Ideapad 1 14igl7 Celeron N4020, 4gb, 128gb , Win11 Color Gris</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>3,328</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Laptop Touch Lenovo Slim 3 I3-1305u 8gb 512gb Ssd W11h 15.6 Color Gris Artico</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8,499</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Laptop Hp 245 G9 Amd Ryzen 3 3250u 8gb Ssd 256gb 14 Hd W11h</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>5,298</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Laptop Gamer Rtx3050 Machenike S15 I5 12450h Ddr4 16g 512g Color Negro Win 11 Pro</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>14,335</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>RTX4060 Portátil Gamer Machenike L16 pro 16'' 2.5K QHD 165Hz I5-13500h 16g 512g Win 11 Pro Laptop</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>17,979</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad 3 15.6'' Ryzen 7 16gb Ram 512gb Ssd Color Sand</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>11,299</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>M2 (2022) 13.6" midnight 8GB de Ram - 256GB SSD - Apple</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>18,623</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Notebook 911X 15.6" gris oscuro 16GB de Ram - 512GB SSD - Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>20,332</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Laptop Hp 240 G8 Intel Core I3 8gb Ram 512gb Ssd 14 Color Negro</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>5,879</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Laptop Huawei Matebook D 16 I5 12th 16gb 512gb Ssd Win11</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>13,499</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Laptop Hp 240 G9 Intel Core I3-1215u 12va Generación, 16gb Ram, 256gb Ssd, Windows 11 Home. Teclado En Español 14 Pulgadas Hd.</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>6,199</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad 1 Ryzen 3 7320u 8gb 256gb Ssd M.2 15.6</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>6,775</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Gamer Ryzen 5 8gb 512gb Win11 Rtx2050 Diginet Color Gris</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>12,249</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>14.1 Hd Laptop Intel Celeron 8gb Ram + 512gb Ssd Windows 11</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>3,626</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Apple MacBook Air (13 pulgadas, 2020, Chip M1, 256 GB de SSD, 8 GB de RAM) - Oro</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>13,294</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Laptop Asus Vivobook Go 15 E1504 Intel Ci3 8gb 512gb Ssd Color Plata</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>7,475</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>I9-13900hx Portátil Gamer Machenike L16 pro Rtx4060 16'' QHD 2560x1600 240Hz Ddr5 16g RAM 1tb SSD Laptop</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>26,093</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Notebook Ultra Slim GWNR51416 14.1" green 8GB de Ram - 256GB SSD - AMD Ryzen 5</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>5,499</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad 3 Intel Ci3 8gb 256ssd Windows 11 Color Frost blue</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>6,799</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Laptop 14'', Intel Celeron N4100 8gb Ram 256gb Ssd W11</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>3,645</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Laptop Hp 14-dq0526la Intel Celeron 4gb 128gb + Impresora</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>5,099</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Notebook Inspiron 3520 15.6" plateado 16GB de Ram - 512GB SSD - Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>10,199</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Laptop Lenovo Ideapad Slim 5 Amd Ryzen 5 7530u, 16gb Ram, 512gb Ssd, Windows 11 Home 64-bit, Wuxga, Teclado En Español Retroiluminado, Gris</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>8,854</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Laptop Hp 245 G9 Ryzen 3 3250u 8gb M.2 512gb Ssd 14 7f213lt Color Negro</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>5,474</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Laptop HP 15-fd0000la 15.6'' Intel Core i3, 8 GB, 512 GB, 15.6, azul</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>7,930</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Notebook Ultra Slim GWNR51416 14.1" azul 8GB de Ram - 256GB SSD - AMD Ryzen 5</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>5,499</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Laptop Huawei Matebook D 14 Ci3 12a 8 Gb 256 Gb Win11 Gris</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>7,999</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Laptop Gamer Lenovo Loq, Ryzen 7 7840h 8gb Ram Ddr5 512 Ssd M.2 Nvidia Rtx 4050 6gb Gddr6, 15.6 Pulgads Full Hd, 144hz, Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>17,599</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Netbook Chuwi PowerBook HeroBook Pro Space Gray 14.1" Intel Celeron N4000 8GB de RAM 256GB SSD 1920x1080px Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>3,773</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>mercadolibre</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Laptop Huawei Matebook D16 I5 12a 8gb 512gb Ssd Windows 11</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>11,199</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
         <is>
           <t>mercadolibre</t>
         </is>

</xml_diff>